<commit_message>
finalize version 1 of the software
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3AC411-653A-4F2B-9063-549AD1B50231}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B36A677-0236-4476-A7F1-4C1BBE440C21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
-  <si>
-    <t>NA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>node_id</t>
   </si>
@@ -92,18 +89,6 @@
   </si>
   <si>
     <t>mode</t>
-  </si>
-  <si>
-    <t>n_grid_at_a_side</t>
-  </si>
-  <si>
-    <t>n_areas_of_different_types</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>block</t>
   </si>
   <si>
     <t>note</t>
@@ -262,26 +247,61 @@
     <t>[42, 48]</t>
   </si>
   <si>
-    <t>required any time (case_instance_generation, single_run, combinatorial_run)</t>
+    <t>fire_degradation_rate_min</t>
   </si>
   <si>
-    <t>single_run</t>
+    <t>fire_degradation_rate_max</t>
+  </si>
+  <si>
+    <t>region_value_min</t>
+  </si>
+  <si>
+    <t>region_value_max</t>
+  </si>
+  <si>
+    <t>required any time (instance_generation, single_run, combinatorial_run)</t>
+  </si>
+  <si>
+    <t>number_of_grids_at_a_side</t>
+  </si>
+  <si>
+    <t>number_of_areas_of_different_types</t>
+  </si>
+  <si>
+    <t>include_water</t>
+  </si>
+  <si>
+    <t>include_block</t>
+  </si>
+  <si>
+    <t>number_of_initial_fires</t>
+  </si>
+  <si>
+    <t>instance_generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -311,12 +331,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,11 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -617,34 +635,34 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -657,23 +675,23 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>2.4676861599938524</v>
-      </c>
-      <c r="F2" s="4">
-        <v>7.8417582417582414</v>
-      </c>
-      <c r="G2" s="4">
-        <v>3.6008073559093967</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1.8320748215604199</v>
+      </c>
+      <c r="F2">
+        <v>5.3360000000000003</v>
+      </c>
+      <c r="G2">
+        <v>2.79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -684,25 +702,25 @@
         <v>0.5</v>
       </c>
       <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7.6273291925465845</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2.6989010989010991</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1.0632034632034633</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.45508679023242</v>
+      </c>
+      <c r="F3">
+        <v>4.6879999999999997</v>
+      </c>
+      <c r="G3">
+        <v>2.11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -713,25 +731,25 @@
         <v>0.5</v>
       </c>
       <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <v>13.196165536591069</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3.6483516483516487</v>
-      </c>
-      <c r="G4" s="4">
-        <v>2.0673992673992676</v>
-      </c>
-      <c r="H4">
+        <v>1.90185873028042</v>
+      </c>
+      <c r="E4">
+        <v>1.07134104210082</v>
+      </c>
+      <c r="F4">
+        <v>1.52</v>
+      </c>
+      <c r="G4">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -742,25 +760,25 @@
         <v>0.5</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.5217582417582418</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5.0725274725274723</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2.173940345368917</v>
-      </c>
-      <c r="H5">
+        <v>1.7623711476334301</v>
+      </c>
+      <c r="E5">
+        <v>2.7923764294318101</v>
+      </c>
+      <c r="F5">
+        <v>4.76</v>
+      </c>
+      <c r="G5">
+        <v>2.375</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -773,20 +791,20 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>2.0254648305281213</v>
-      </c>
-      <c r="F6" s="4">
-        <v>6.5758241758241756</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2.9270436880192974</v>
-      </c>
-      <c r="H6">
+      <c r="E6">
+        <v>2.18521516917101</v>
+      </c>
+      <c r="F6">
+        <v>6.4880000000000004</v>
+      </c>
+      <c r="G6">
+        <v>3.2949999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
         <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -800,25 +818,25 @@
         <v>0.5</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.0073260073260073</v>
-      </c>
-      <c r="F7" s="4">
-        <v>6.0219780219780219</v>
-      </c>
-      <c r="G7" s="4">
-        <v>3.0109890109890109</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.9072673696128999</v>
+      </c>
+      <c r="E7">
+        <v>5.93063107630317</v>
+      </c>
+      <c r="F7">
+        <v>5.84</v>
+      </c>
+      <c r="G7">
+        <v>3.1349999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -831,20 +849,20 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <v>2.035689081560641</v>
-      </c>
-      <c r="F8" s="4">
-        <v>5.5472527472527471</v>
-      </c>
-      <c r="G8" s="4">
-        <v>3.215798694059564</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>35</v>
+      <c r="E8">
+        <v>1.8788732394366101</v>
+      </c>
+      <c r="F8">
+        <v>5.3360000000000003</v>
+      </c>
+      <c r="G8">
+        <v>2.9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -858,25 +876,25 @@
         <v>1.5</v>
       </c>
       <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>16.68029860434924</v>
-      </c>
-      <c r="F9" s="4">
-        <v>6.4175824175824179</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.0884615384615381</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.5018343336139903</v>
+      </c>
+      <c r="E9">
+        <v>2.3313206097205601</v>
+      </c>
+      <c r="F9">
+        <v>0.872</v>
+      </c>
+      <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -887,25 +905,25 @@
         <v>1.5</v>
       </c>
       <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>14.886211276161022</v>
-      </c>
-      <c r="F10" s="4">
-        <v>5.0725274725274723</v>
-      </c>
-      <c r="G10" s="4">
-        <v>2.9388452817024242</v>
-      </c>
-      <c r="H10">
+        <v>6.4438099060036498</v>
+      </c>
+      <c r="E10">
+        <v>6.3615734988167301</v>
+      </c>
+      <c r="F10">
+        <v>2.8879999999999999</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -916,22 +934,22 @@
         <v>1.5</v>
       </c>
       <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>4.5800053604931659</v>
-      </c>
-      <c r="F11" s="4">
-        <v>6.2593406593406602</v>
-      </c>
-      <c r="G11" s="4">
-        <v>3.6111580726965347</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>38</v>
+        <v>1.63088628244763</v>
+      </c>
+      <c r="E11">
+        <v>2.2460808408121302</v>
+      </c>
+      <c r="F11">
+        <v>4.3280000000000003</v>
+      </c>
+      <c r="G11">
+        <v>2.02</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -945,22 +963,22 @@
         <v>1.5</v>
       </c>
       <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.625856496444732</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2.3032967032967036</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.49356357927786504</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>39</v>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2.3295370908386501</v>
+      </c>
+      <c r="F12">
+        <v>6.7759999999999998</v>
+      </c>
+      <c r="G12">
+        <v>3.55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -974,25 +992,25 @@
         <v>1.5</v>
       </c>
       <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13" s="2">
-        <v>4.5069135588820632</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3.4901098901098901</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1.6638895987733195</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2.4894652219503599</v>
+      </c>
+      <c r="F13">
+        <v>7.7839999999999998</v>
+      </c>
+      <c r="G13">
+        <v>3.66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1002,26 +1020,26 @@
       <c r="C14">
         <v>1.5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>3.9905992068137799</v>
+      </c>
+      <c r="E14">
+        <v>8.36172218209364</v>
+      </c>
+      <c r="F14">
+        <v>6.2</v>
+      </c>
+      <c r="G14">
+        <v>3.165</v>
+      </c>
+      <c r="H14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1032,22 +1050,22 @@
         <v>1.5</v>
       </c>
       <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15" s="2">
-        <v>7.7622948480091338</v>
-      </c>
-      <c r="F15" s="4">
-        <v>6.4967032967032976</v>
-      </c>
-      <c r="G15" s="4">
-        <v>2.7671143671143672</v>
-      </c>
-      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1.308868249054</v>
+      </c>
+      <c r="F15">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="G15">
+        <v>1.99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15">
         <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1061,25 +1079,25 @@
         <v>2.5</v>
       </c>
       <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.96000000000000019</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.15528623168845</v>
+      </c>
+      <c r="E16">
+        <v>4.5829478175020704</v>
+      </c>
+      <c r="F16">
+        <v>3.2480000000000002</v>
+      </c>
+      <c r="G16">
+        <v>1.67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1090,25 +1108,25 @@
         <v>2.5</v>
       </c>
       <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2.9251245648761182</v>
-      </c>
-      <c r="F17" s="4">
-        <v>4.2813186813186821</v>
-      </c>
-      <c r="G17" s="4">
-        <v>2.221438938420071</v>
-      </c>
-      <c r="H17">
+        <v>6.60138016741484</v>
+      </c>
+      <c r="E17">
+        <v>4.7588471610812197</v>
+      </c>
+      <c r="F17">
+        <v>2.1680000000000001</v>
+      </c>
+      <c r="G17">
+        <v>1.08</v>
+      </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1119,25 +1137,25 @@
         <v>2.5</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3.1203296703296708</v>
-      </c>
-      <c r="F18" s="4">
-        <v>5.5472527472527471</v>
-      </c>
-      <c r="G18" s="4">
-        <v>2.1706641184902056</v>
-      </c>
-      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1.57446537235583</v>
+      </c>
+      <c r="F18">
+        <v>4.4720000000000004</v>
+      </c>
+      <c r="G18">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1148,25 +1166,25 @@
         <v>2.5</v>
       </c>
       <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2">
-        <v>4.1494505494505507</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1.0373626373626375</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0.69157509157509167</v>
-      </c>
-      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1.66469945355191</v>
+      </c>
+      <c r="F19">
+        <v>4.76</v>
+      </c>
+      <c r="G19">
+        <v>2.56</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19">
         <v>0</v>
       </c>
-      <c r="I19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1177,25 +1195,25 @@
         <v>2.5</v>
       </c>
       <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2">
-        <v>7.384615384615385</v>
-      </c>
-      <c r="F20" s="4">
-        <v>3.0153846153846153</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0.97796257796257791</v>
-      </c>
-      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1.57771483045076</v>
+      </c>
+      <c r="F20">
+        <v>5.048</v>
+      </c>
+      <c r="G20">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
-      <c r="I20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1205,23 +1223,23 @@
       <c r="C21">
         <v>2.5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>6.2679836758742802</v>
+      </c>
+      <c r="E21">
+        <v>5.8261017212506498</v>
+      </c>
+      <c r="F21">
+        <v>2.96</v>
+      </c>
+      <c r="G21">
+        <v>1.355</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21">
         <v>0</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-      <c r="I21" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1235,25 +1253,25 @@
         <v>2.5</v>
       </c>
       <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2.7777843777843776</v>
-      </c>
-      <c r="F22" s="4">
-        <v>3.8065934065934064</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2.1867664250642975</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.57086220789685704</v>
+      </c>
+      <c r="F22">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.89</v>
+      </c>
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1266,23 +1284,23 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="2">
-        <v>2.4997802197802197</v>
-      </c>
-      <c r="F23" s="4">
-        <v>7.4461538461538463</v>
-      </c>
-      <c r="G23" s="4">
-        <v>3.763110008271298</v>
-      </c>
-      <c r="H23">
+      <c r="E23">
+        <v>1.51377751687701</v>
+      </c>
+      <c r="F23">
+        <v>4.5439999999999996</v>
+      </c>
+      <c r="G23">
+        <v>2.27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1295,23 +1313,23 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="2">
-        <v>2.2624332189549583</v>
-      </c>
-      <c r="F24" s="4">
-        <v>6.7340659340659341</v>
-      </c>
-      <c r="G24" s="4">
-        <v>3.4071166928309786</v>
-      </c>
-      <c r="H24">
+      <c r="E24">
+        <v>1.66914115415876</v>
+      </c>
+      <c r="F24">
+        <v>4.8319999999999999</v>
+      </c>
+      <c r="G24">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="I24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1322,25 +1340,25 @@
         <v>3.5</v>
       </c>
       <c r="D25">
+        <v>-1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25">
         <v>4</v>
       </c>
-      <c r="E25" s="2">
-        <v>9.1846238053134606</v>
-      </c>
-      <c r="F25" s="4">
-        <v>7.0505494505494504</v>
-      </c>
-      <c r="G25" s="4">
-        <v>3.4050949050949049</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1351,25 +1369,25 @@
         <v>3.5</v>
       </c>
       <c r="D26">
+        <v>-1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26">
         <v>4</v>
       </c>
-      <c r="E26" s="2">
-        <v>5.3823129251700674</v>
-      </c>
-      <c r="F26" s="4">
-        <v>4.9142857142857137</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1.852927400468384</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1382,20 +1400,20 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="2">
-        <v>1.3257142857142856</v>
-      </c>
-      <c r="F27" s="4">
-        <v>3.569230769230769</v>
-      </c>
-      <c r="G27" s="4">
-        <v>2.1090909090909089</v>
-      </c>
-      <c r="H27">
+      <c r="E27">
+        <v>2.0541896289867601</v>
+      </c>
+      <c r="F27">
+        <v>6.1280000000000001</v>
+      </c>
+      <c r="G27">
+        <v>3.09</v>
+      </c>
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27">
         <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1409,25 +1427,25 @@
         <v>3.5</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2.1565795548988831</v>
-      </c>
-      <c r="F28" s="4">
-        <v>6.2593406593406602</v>
-      </c>
-      <c r="G28" s="4">
-        <v>3.290166244012398</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.0840450635204801</v>
+      </c>
+      <c r="E28">
+        <v>7.2177397762015403</v>
+      </c>
+      <c r="F28">
+        <v>3.32</v>
+      </c>
+      <c r="G28">
+        <v>1.47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1438,25 +1456,25 @@
         <v>3.5</v>
       </c>
       <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2.1930279458369344</v>
-      </c>
-      <c r="F29" s="4">
-        <v>7.604395604395604</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3.0817813765182187</v>
-      </c>
-      <c r="H29">
+        <v>6.3191286924153696</v>
+      </c>
+      <c r="E29">
+        <v>5.7197582126817501</v>
+      </c>
+      <c r="F29">
+        <v>2.528</v>
+      </c>
+      <c r="G29">
+        <v>1.41</v>
+      </c>
+      <c r="H29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29">
         <v>0</v>
       </c>
-      <c r="I29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1467,25 +1485,25 @@
         <v>4.5</v>
       </c>
       <c r="D30">
-        <v>8</v>
-      </c>
-      <c r="E30" s="2">
-        <v>11.13766233766234</v>
-      </c>
-      <c r="F30" s="4">
-        <v>4.1230769230769235</v>
-      </c>
-      <c r="G30" s="4">
-        <v>2.101960784313726</v>
-      </c>
-      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1.91572490267783</v>
+      </c>
+      <c r="F30">
+        <v>5.5519999999999996</v>
+      </c>
+      <c r="G30">
+        <v>2.9249999999999998</v>
+      </c>
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30">
         <v>0</v>
       </c>
-      <c r="I30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1496,25 +1514,25 @@
         <v>4.5</v>
       </c>
       <c r="D31">
-        <v>10</v>
-      </c>
-      <c r="E31" s="2">
-        <v>25.507692307692309</v>
-      </c>
-      <c r="F31" s="4">
-        <v>7.2879120879120878</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3.9242603550295856</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>2.26178988326848</v>
+      </c>
+      <c r="F31">
+        <v>6.92</v>
+      </c>
+      <c r="G31">
+        <v>3.36</v>
+      </c>
+      <c r="H31" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1525,25 +1543,25 @@
         <v>4.5</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0.29416737109044805</v>
-      </c>
-      <c r="F32" s="4">
-        <v>1.2747252747252749</v>
-      </c>
-      <c r="G32" s="4">
-        <v>0.38241758241758245</v>
-      </c>
-      <c r="H32">
+        <v>1.25069065841635</v>
+      </c>
+      <c r="E32">
+        <v>2.2717444978210999</v>
+      </c>
+      <c r="F32">
+        <v>5.4080000000000004</v>
+      </c>
+      <c r="G32">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32">
         <v>0</v>
       </c>
-      <c r="I32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1554,25 +1572,25 @@
         <v>4.5</v>
       </c>
       <c r="D33">
-        <v>10</v>
-      </c>
-      <c r="E33" s="2">
-        <v>25.08424908424908</v>
-      </c>
-      <c r="F33" s="4">
-        <v>7.5252747252747243</v>
-      </c>
-      <c r="G33" s="4">
-        <v>3.7626373626373621</v>
-      </c>
-      <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1583,25 +1601,25 @@
         <v>4.5</v>
       </c>
       <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2">
-        <v>2.0666790836282365</v>
-      </c>
-      <c r="F34" s="4">
-        <v>6.4175824175824179</v>
-      </c>
-      <c r="G34" s="4">
-        <v>3.0483516483516486</v>
-      </c>
-      <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1612,25 +1630,25 @@
         <v>4.5</v>
       </c>
       <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2">
-        <v>2.2180896027049877</v>
-      </c>
-      <c r="F35" s="4">
-        <v>7.2087912087912089</v>
-      </c>
-      <c r="G35" s="4">
-        <v>3.2039072039072041</v>
-      </c>
-      <c r="H35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>16.851879797059901</v>
+      </c>
+      <c r="F35">
+        <v>5.1920000000000002</v>
+      </c>
+      <c r="G35">
+        <v>2.4950000000000001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35">
         <v>0</v>
       </c>
-      <c r="I35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1641,22 +1659,22 @@
         <v>4.5</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2">
-        <v>2.6127946127946124</v>
-      </c>
-      <c r="F36" s="4">
-        <v>8</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3.8799999999999994</v>
-      </c>
-      <c r="H36">
+        <v>-1</v>
+      </c>
+      <c r="E36">
         <v>0</v>
       </c>
-      <c r="I36" t="s">
-        <v>63</v>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1670,25 +1688,25 @@
         <v>5.5</v>
       </c>
       <c r="D37">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2">
-        <v>10.922007722007722</v>
-      </c>
-      <c r="F37" s="4">
-        <v>3.8857142857142852</v>
-      </c>
-      <c r="G37" s="4">
-        <v>2.1047619047619048</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>2.0982477967858899</v>
+      </c>
+      <c r="F37">
+        <v>6.56</v>
+      </c>
+      <c r="G37">
+        <v>3.085</v>
+      </c>
+      <c r="H37" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1699,25 +1717,25 @@
         <v>5.5</v>
       </c>
       <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" s="2">
-        <v>2.6540196645459799</v>
-      </c>
-      <c r="F38" s="4">
-        <v>4.2021978021978024</v>
-      </c>
-      <c r="G38" s="4">
-        <v>1.9394759087066777</v>
-      </c>
-      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1.63172322022621</v>
+      </c>
+      <c r="F38">
+        <v>5.12</v>
+      </c>
+      <c r="G38">
+        <v>2.395</v>
+      </c>
+      <c r="H38" t="s">
+        <v>60</v>
+      </c>
+      <c r="I38">
         <v>0</v>
       </c>
-      <c r="I38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1728,25 +1746,25 @@
         <v>5.5</v>
       </c>
       <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="2">
-        <v>0.78321678321678323</v>
-      </c>
-      <c r="F39" s="4">
-        <v>2.4615384615384617</v>
-      </c>
-      <c r="G39" s="4">
-        <v>1.1487179487179489</v>
-      </c>
-      <c r="H39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>9.0742777906170495</v>
+      </c>
+      <c r="F39">
+        <v>3.032</v>
+      </c>
+      <c r="G39">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="H39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I39">
         <v>0</v>
       </c>
-      <c r="I39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1757,25 +1775,25 @@
         <v>5.5</v>
       </c>
       <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2">
-        <v>1.5247739602169981</v>
-      </c>
-      <c r="F40" s="4">
-        <v>3.8857142857142852</v>
-      </c>
-      <c r="G40" s="4">
-        <v>2.5095238095238095</v>
-      </c>
-      <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>62</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1786,25 +1804,25 @@
         <v>5.5</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2">
-        <v>2.4375505535356838</v>
-      </c>
-      <c r="F41" s="4">
-        <v>7.0505494505494504</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3.7255744255744259</v>
-      </c>
-      <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1815,25 +1833,25 @@
         <v>5.5</v>
       </c>
       <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1.6782554233331433</v>
-      </c>
-      <c r="F42" s="4">
-        <v>5.3098901098901097</v>
-      </c>
-      <c r="G42" s="4">
-        <v>2.4538128538128534</v>
-      </c>
-      <c r="H42">
-        <v>4</v>
-      </c>
-      <c r="I42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.6047603713525098</v>
+      </c>
+      <c r="E42">
+        <v>2.7052949821766399</v>
+      </c>
+      <c r="F42">
+        <v>2.96</v>
+      </c>
+      <c r="G42">
+        <v>1.6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1846,20 +1864,20 @@
       <c r="D43">
         <v>1</v>
       </c>
-      <c r="E43" s="2">
-        <v>2.1920137475693031</v>
-      </c>
-      <c r="F43" s="4">
-        <v>6.4175824175824179</v>
-      </c>
-      <c r="G43" s="4">
-        <v>3.3291208791208788</v>
-      </c>
-      <c r="H43">
+      <c r="E43">
+        <v>2.1616535758577902</v>
+      </c>
+      <c r="F43">
+        <v>6.4160000000000004</v>
+      </c>
+      <c r="G43">
+        <v>3.26</v>
+      </c>
+      <c r="H43" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43">
         <v>0</v>
-      </c>
-      <c r="I43" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1872,26 +1890,26 @@
       <c r="C44">
         <v>6.5</v>
       </c>
-      <c r="D44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>6</v>
-      </c>
-      <c r="I44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>2.6586183769282301</v>
+      </c>
+      <c r="F44">
+        <v>7.9279999999999999</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1902,22 +1920,22 @@
         <v>6.5</v>
       </c>
       <c r="D45">
-        <v>10</v>
-      </c>
-      <c r="E45" s="2">
-        <v>7.7729742784687845</v>
-      </c>
-      <c r="F45" s="4">
-        <v>2.6197802197802198</v>
-      </c>
-      <c r="G45" s="4">
-        <v>1.1052197802197803</v>
-      </c>
-      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1.63821835958718</v>
+      </c>
+      <c r="F45">
+        <v>4.9039999999999999</v>
+      </c>
+      <c r="G45">
+        <v>2.46</v>
+      </c>
+      <c r="H45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45">
         <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1933,20 +1951,20 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46" s="2">
-        <v>1.9669869879074895</v>
-      </c>
-      <c r="F46" s="4">
-        <v>6.813186813186813</v>
-      </c>
-      <c r="G46" s="4">
-        <v>2.765352294764059</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
-        <v>73</v>
+      <c r="E46">
+        <v>1.6453992084072599</v>
+      </c>
+      <c r="F46">
+        <v>4.8319999999999999</v>
+      </c>
+      <c r="G46">
+        <v>2.4950000000000001</v>
+      </c>
+      <c r="H46" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -1962,23 +1980,23 @@
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="2">
-        <v>2.1032412965186076</v>
-      </c>
-      <c r="F47" s="4">
-        <v>6.4175824175824179</v>
-      </c>
-      <c r="G47" s="4">
-        <v>3.1285714285714281</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>2.3459994356128302</v>
+      </c>
+      <c r="F47">
+        <v>7.1360000000000001</v>
+      </c>
+      <c r="G47">
+        <v>3.4950000000000001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1989,25 +2007,25 @@
         <v>6.5</v>
       </c>
       <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2">
-        <v>2.2045987625819565</v>
-      </c>
-      <c r="F48" s="4">
-        <v>6.1010989010989016</v>
-      </c>
-      <c r="G48" s="4">
-        <v>3.4519375361480629</v>
-      </c>
-      <c r="H48">
+        <v>2.5472706288413498</v>
+      </c>
+      <c r="E48">
+        <v>1.9244704963932799</v>
+      </c>
+      <c r="F48">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="G48">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H48" t="s">
+        <v>70</v>
+      </c>
+      <c r="I48">
         <v>0</v>
       </c>
-      <c r="I48" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2018,22 +2036,22 @@
         <v>6.5</v>
       </c>
       <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2">
-        <v>2.0250899542934939</v>
-      </c>
-      <c r="F49" s="4">
-        <v>6.0219780219780219</v>
-      </c>
-      <c r="G49" s="4">
-        <v>3.051135531135531</v>
-      </c>
-      <c r="H49">
+        <v>2.4267416109790401</v>
+      </c>
+      <c r="E49">
+        <v>0.69648855275556698</v>
+      </c>
+      <c r="F49">
+        <v>1.016</v>
+      </c>
+      <c r="G49">
+        <v>0.4</v>
+      </c>
+      <c r="H49" t="s">
+        <v>71</v>
+      </c>
+      <c r="I49">
         <v>0</v>
-      </c>
-      <c r="I49" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2047,28 +2065,35 @@
         <v>6.5</v>
       </c>
       <c r="D50">
-        <v>2</v>
-      </c>
-      <c r="E50" s="2">
-        <v>0.66780925496521826</v>
-      </c>
-      <c r="F50" s="4">
-        <v>4.0439560439560438</v>
-      </c>
-      <c r="G50" s="4">
-        <v>0.36395604395604397</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D51" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>2.1281153450051402</v>
+      </c>
+      <c r="F50">
+        <v>6.56</v>
+      </c>
+      <c r="G50">
+        <v>3.15</v>
+      </c>
+      <c r="H50" t="s">
+        <v>72</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I51" xr:uid="{70FEF19A-E29D-444F-91B6-49EF351C9362}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2088,13 +2113,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -27911,105 +27936,105 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C388623-1A6B-40E9-8627-160DBCAB28EA}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -28019,46 +28044,89 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to instance genertor
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00746CF-F641-47DD-9547-515ADD1C68B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDF0B8E-FC0A-4979-9BBD-8A9B103D5336}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>required any time (instance_generation, single_run, combination_run)</t>
   </si>
   <si>
-    <t>combination_run</t>
+    <t>instance_generation</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding default_density as user input
I added two parameters in the excel sheet called default_housing_density and default_vegetation_density so users can use this to input the default density
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDF0B8E-FC0A-4979-9BBD-8A9B103D5336}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CCAD21-FC08-46DA-A813-E54797E1F101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_df" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>NA</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>instance_generation</t>
+  </si>
+  <si>
+    <t>required for case instance; 0 if &lt;50% vegetated, 1 if &gt;50% vegetated</t>
+  </si>
+  <si>
+    <t>default_housing_density</t>
+  </si>
+  <si>
+    <t>default_vegetation_density</t>
+  </si>
+  <si>
+    <t>required for case instance; in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741</t>
   </si>
 </sst>
 </file>
@@ -541,19 +553,19 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -582,7 +594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -611,7 +623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -640,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -669,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -698,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -727,7 +739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -756,7 +768,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -785,7 +797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -814,7 +826,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -843,7 +855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -872,7 +884,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -901,7 +913,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -930,7 +942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -959,7 +971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -988,7 +1000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1046,7 +1058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1075,7 +1087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1191,7 +1203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1249,7 +1261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1314,20 +1326,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C388623-1A6B-40E9-8627-160DBCAB28EA}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1349,7 +1361,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1360,7 +1372,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1383,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1382,7 +1394,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1415,12 +1427,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1431,7 +1443,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1442,7 +1454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1453,7 +1465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1475,35 +1487,57 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B15">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
folder organization before public share
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A21A91-58A5-4C93-9D80-BC3B98CF41F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720B8D3E-DDAD-4C7B-9186-A85DAE3198AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_df" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>NA</t>
   </si>
@@ -158,15 +158,9 @@
     <t>note</t>
   </si>
   <si>
-    <t>required for MIP</t>
-  </si>
-  <si>
     <t>number_of_initial_fires</t>
   </si>
   <si>
-    <t>required for case instance</t>
-  </si>
-  <si>
     <t>number_of_grids_at_a_side</t>
   </si>
   <si>
@@ -191,22 +185,45 @@
     <t>region_value_max</t>
   </si>
   <si>
-    <t>required any time (instance_generation, single_run, combination_run)</t>
-  </si>
-  <si>
-    <t>instance_generation</t>
-  </si>
-  <si>
-    <t>required for case instance; 0 if &lt;50% vegetated, 1 if &gt;50% vegetated</t>
+    <t>requirements</t>
+  </si>
+  <si>
+    <t>required for single_run and combination_run modes</t>
+  </si>
+  <si>
+    <t>required for instance_generation mode</t>
+  </si>
+  <si>
+    <t>defines region size (e.g 7 sets  7x7 region)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>??? Should we ignore this?
+Do we have control on the number of water resources?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: no fire proof nodes, 1: add fire proof nodes
+do we have control on the number of blocks? </t>
   </si>
   <si>
     <t>default_housing_density</t>
   </si>
   <si>
+    <t>in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741</t>
+  </si>
+  <si>
     <t>default_vegetation_density</t>
   </si>
   <si>
-    <t>required for case instance; in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741</t>
+    <t>0 if &lt;50% vegetated, 1 if &gt;50% vegetated</t>
+  </si>
+  <si>
+    <t>instance_generation, single_run, combination_run</t>
+  </si>
+  <si>
+    <t>single_run</t>
   </si>
 </sst>
 </file>
@@ -257,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -265,8 +282,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,23 +576,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -594,7 +619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -623,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -652,7 +677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -681,7 +706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -710,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -739,7 +764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -768,7 +793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -797,7 +822,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -826,7 +851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -855,7 +880,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -884,7 +909,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -913,7 +938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -942,7 +967,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -971,7 +996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1000,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1029,7 +1054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1058,7 +1083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1087,7 +1112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1116,7 +1141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1145,7 +1170,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1174,7 +1199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1203,7 +1228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1232,7 +1257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1261,7 +1286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1290,7 +1315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1326,20 +1351,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C388623-1A6B-40E9-8627-160DBCAB28EA}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1349,196 +1374,247 @@
       <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>120</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="4">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D11" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="4">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a major change to case_generator_setup.py by Esther
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D07988A-2413-4766-800B-19242D6C227E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CEA84D-CD49-4664-91DE-44FACEDDEF59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_df" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>NA</t>
   </si>
@@ -161,18 +161,15 @@
     <t>number_of_initial_fires</t>
   </si>
   <si>
+    <t>required for case instance</t>
+  </si>
+  <si>
     <t>number_of_grids_at_a_side</t>
   </si>
   <si>
     <t>number_of_areas_of_different_types</t>
   </si>
   <si>
-    <t>include_water</t>
-  </si>
-  <si>
-    <t>include_block</t>
-  </si>
-  <si>
     <t>fire_degradation_rate_min</t>
   </si>
   <si>
@@ -185,45 +182,37 @@
     <t>region_value_max</t>
   </si>
   <si>
-    <t>requirements</t>
-  </si>
-  <si>
-    <t>required for single_run and combination_run modes</t>
-  </si>
-  <si>
-    <t>required for instance_generation mode</t>
-  </si>
-  <si>
-    <t>defines region size (e.g 7 sets  7x7 region)</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>??? Should we ignore this?
-Do we have control on the number of water resources?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0: no fire proof nodes, 1: add fire proof nodes
-do we have control on the number of blocks? </t>
+    <t>required any time (instance_generation, single_run, combination_run)</t>
   </si>
   <si>
     <t>default_housing_density</t>
   </si>
   <si>
-    <t>in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741</t>
-  </si>
-  <si>
     <t>default_vegetation_density</t>
   </si>
   <si>
-    <t>0 if &lt;50% vegetated, 1 if &gt;50% vegetated</t>
-  </si>
-  <si>
-    <t>instance_generation, single_run, combination_run</t>
-  </si>
-  <si>
-    <t>single_run</t>
+    <t>number_of_water_bodies</t>
+  </si>
+  <si>
+    <t>number_of_blocks</t>
+  </si>
+  <si>
+    <t>required for case instance (must be greater than 0)</t>
+  </si>
+  <si>
+    <t>required for case instance; in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741 (If you want the default type to be water or block: set to 0 or -1 respectively)</t>
+  </si>
+  <si>
+    <t>required for case instance; 0 if &lt;50% vegetated, 1 if &gt;50% vegetated (If you want the default type to be water or block: set to 2 or 3 respectively)</t>
+  </si>
+  <si>
+    <t>required for MIP  for single_run and combination_run modes</t>
+  </si>
+  <si>
+    <t>required for MIP for single_run and combination_run modes</t>
+  </si>
+  <si>
+    <t>instance_generation</t>
   </si>
 </sst>
 </file>
@@ -274,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -282,18 +271,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C388623-1A6B-40E9-8627-160DBCAB28EA}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,7 +1345,7 @@
     <col min="3" max="3" width="64.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1376,247 +1355,208 @@
       <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17">
+        <v>0.4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="4">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="C20" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="4">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="4">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="4">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for paper revision
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CEA84D-CD49-4664-91DE-44FACEDDEF59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68037DA8-7895-45EA-BA13-B9EF72EDB70E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_df" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>NA</t>
   </si>
@@ -152,12 +152,12 @@
     <t>[5, 15, 9]</t>
   </si>
   <si>
-    <t>mode</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
+    <t>required for MIP</t>
+  </si>
+  <si>
     <t>number_of_initial_fires</t>
   </si>
   <si>
@@ -170,6 +170,12 @@
     <t>number_of_areas_of_different_types</t>
   </si>
   <si>
+    <t>include_water</t>
+  </si>
+  <si>
+    <t>include_block</t>
+  </si>
+  <si>
     <t>fire_degradation_rate_min</t>
   </si>
   <si>
@@ -182,37 +188,37 @@
     <t>region_value_max</t>
   </si>
   <si>
-    <t>required any time (instance_generation, single_run, combination_run)</t>
-  </si>
-  <si>
-    <t>default_housing_density</t>
-  </si>
-  <si>
-    <t>default_vegetation_density</t>
-  </si>
-  <si>
-    <t>number_of_water_bodies</t>
-  </si>
-  <si>
-    <t>number_of_blocks</t>
-  </si>
-  <si>
-    <t>required for case instance (must be greater than 0)</t>
-  </si>
-  <si>
-    <t>required for case instance; in units/sq km, 1: 0; 2: &lt;6; 3: 6-50; 4: 50-741; 5: &gt; 741 (If you want the default type to be water or block: set to 0 or -1 respectively)</t>
-  </si>
-  <si>
-    <t>required for case instance; 0 if &lt;50% vegetated, 1 if &gt;50% vegetated (If you want the default type to be water or block: set to 2 or 3 respectively)</t>
-  </si>
-  <si>
-    <t>required for MIP  for single_run and combination_run modes</t>
-  </si>
-  <si>
-    <t>required for MIP for single_run and combination_run modes</t>
-  </si>
-  <si>
-    <t>instance_generation</t>
+    <t>combination_results_file_name</t>
+  </si>
+  <si>
+    <t>combination-results-2uav-60v-erdi.csv</t>
+  </si>
+  <si>
+    <t>clustering_cost_function</t>
+  </si>
+  <si>
+    <t>value_decrease</t>
+  </si>
+  <si>
+    <t>value_decrease or spread_rate</t>
+  </si>
+  <si>
+    <t>clustering_neighborhood_level</t>
+  </si>
+  <si>
+    <t>clustering_distance_on_off</t>
+  </si>
+  <si>
+    <t>single_run_hybrid_combination_run</t>
+  </si>
+  <si>
+    <t>algorithm</t>
+  </si>
+  <si>
+    <t>experiment_mode</t>
+  </si>
+  <si>
+    <t>required any time. Available models: (instance_generation, single_run, combination_run, combination_run_from_file, cluster_first, cluster_first_combination_run, cluster_first_lean, single_run_lean)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +832,7 @@
         <v>2.96</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
@@ -855,7 +861,7 @@
         <v>1.52</v>
       </c>
       <c r="H10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>41</v>
@@ -1029,7 +1035,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="H16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>25</v>
@@ -1087,7 +1093,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>27</v>
@@ -1232,7 +1238,7 @@
         <v>2.96</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>32</v>
@@ -1332,16 +1338,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C388623-1A6B-40E9-8627-160DBCAB28EA}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1353,108 +1359,102 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -1473,21 +1473,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
@@ -1495,68 +1495,80 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B17">
-        <v>0.4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to include E-RLM
</commit_message>
<xml_diff>
--- a/inputs/inputs_to_load.xlsx
+++ b/inputs/inputs_to_load.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85FDD20-2B55-4424-95C1-41F6F4223EA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE320934-97AF-42A6-8754-E6DCBC426162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_df" sheetId="1" r:id="rId1"/>
@@ -191,6 +191,9 @@
     <t>combination_results_file_name</t>
   </si>
   <si>
+    <t>combination-results-2uav-60v-erdi.csv</t>
+  </si>
+  <si>
     <t>clustering_cost_function</t>
   </si>
   <si>
@@ -222,9 +225,6 @@
   </si>
   <si>
     <t>e-rlm</t>
-  </si>
-  <si>
-    <t>combination-results-2uav-120v.csv</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1347,7 +1347,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,24 +1370,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1439,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
@@ -1550,18 +1550,18 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>